<commit_message>
add test of etl v1
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -460,11 +460,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NB43</t>
+          <t>NB13</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>13328</v>
+        <v>11626</v>
       </c>
     </row>
     <row r="3">
@@ -475,11 +475,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PC1</t>
+          <t>PC20</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>11668</v>
+        <v>7862</v>
       </c>
     </row>
   </sheetData>
@@ -530,13 +530,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13328</v>
+        <v>11626</v>
       </c>
       <c r="C2" t="n">
-        <v>6148</v>
+        <v>8675</v>
       </c>
       <c r="D2" t="n">
-        <v>9395.790000000001</v>
+        <v>9728.33</v>
       </c>
     </row>
     <row r="3">
@@ -546,13 +546,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11668</v>
+        <v>7862</v>
       </c>
       <c r="C3" t="n">
-        <v>4234</v>
+        <v>5854</v>
       </c>
       <c r="D3" t="n">
-        <v>7947.83</v>
+        <v>6858</v>
       </c>
     </row>
   </sheetData>
@@ -603,13 +603,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2000</v>
+        <v>1506</v>
       </c>
       <c r="C2" t="n">
-        <v>1025</v>
+        <v>1136</v>
       </c>
       <c r="D2" t="n">
-        <v>1542.56</v>
+        <v>1291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>